<commit_message>
add datatest example, update slides
</commit_message>
<xml_diff>
--- a/data/test_cais/cais_name_counts_manual_2018-2019.xlsx
+++ b/data/test_cais/cais_name_counts_manual_2018-2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\0.SurfaceOwl\dev\pdf_extract_990\data\test_cais\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\0.SurfaceOwl\dev\pythontalk.tdd_for_data\data\test_cais\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D3AB91-0348-4C62-ADA7-54F1C3B3F5A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1178372B-1E2F-429D-95AE-A58B553A5C05}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10215" yWindow="2385" windowWidth="27480" windowHeight="16875" xr2:uid="{94DC2705-DD5F-4C3A-8482-A8FD55667898}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="32340" windowHeight="14085" xr2:uid="{94DC2705-DD5F-4C3A-8482-A8FD55667898}"/>
   </bookViews>
   <sheets>
     <sheet name="school_name_counts_by_sheet" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
   <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,16 +578,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
-        <v>7</v>
-      </c>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -598,10 +598,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2">
         <v>9</v>
@@ -621,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
@@ -641,7 +641,7 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2">
         <v>9</v>
@@ -661,13 +661,13 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -681,13 +681,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -701,13 +701,13 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2">
         <v>8</v>
       </c>
-      <c r="D8" s="2">
-        <v>10</v>
-      </c>
       <c r="E8" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -721,13 +721,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -741,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2">
         <v>10</v>
@@ -761,16 +761,16 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,13 +781,13 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -801,16 +801,16 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E13" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -821,16 +821,16 @@
         <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2">
         <v>9</v>
       </c>
       <c r="E14" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F14" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -841,16 +841,16 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -861,13 +861,13 @@
         <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D16" s="2">
         <v>9</v>
       </c>
       <c r="E16" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2">
         <v>9</v>
@@ -890,7 +890,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -901,16 +901,16 @@
         <v>0</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -921,16 +921,16 @@
         <v>0</v>
       </c>
       <c r="C19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -941,16 +941,16 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E20" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F20" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,16 +961,16 @@
         <v>0</v>
       </c>
       <c r="C21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D21" s="2">
         <v>8</v>
       </c>
       <c r="E21" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F21" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -981,16 +981,16 @@
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D22" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,16 +1001,16 @@
         <v>0</v>
       </c>
       <c r="C23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D23" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F23" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1021,16 +1021,16 @@
         <v>0</v>
       </c>
       <c r="C24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D24" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E24" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F24" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1041,16 +1041,16 @@
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,19 +1058,19 @@
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D26" s="2">
+        <v>9</v>
+      </c>
+      <c r="E26" s="2">
+        <v>3</v>
+      </c>
+      <c r="F26" s="2">
         <v>2</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1078,19 +1078,19 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D27" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E27" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>